<commit_message>
Reworked test cases - (Task #329)
- Made validation calls a part of the import test cases

---
Task #329: Excel import always results in NPE
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.funcelectrical.test/resources/ImportElementDefinitionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.funcelectrical.test/resources/ImportElementDefinitionTest.xlsx
@@ -121,16 +121,16 @@
     <t>POW_NEW</t>
   </si>
   <si>
-    <t>74ccc93a-281b-4ab8-ace4-cb7f2b9827d4b</t>
-  </si>
-  <si>
-    <t>BATTERY1</t>
-  </si>
-  <si>
     <t>supe_us</t>
   </si>
   <si>
     <t>16:21 18/7/2016</t>
+  </si>
+  <si>
+    <t>74ccc93a-281b-4ab8-acec-b7f2b9827d4b</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2"/>
     </row>

</xml_diff>